<commit_message>
Fixed FadeOut before next FX
</commit_message>
<xml_diff>
--- a/PhotonTorpedo.Particle/Calculations.xlsx
+++ b/PhotonTorpedo.Particle/Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rainbow" sheetId="1" r:id="rId1"/>
@@ -81,15 +81,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -106,12 +112,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -126,6 +203,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +273,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2626,11 +2714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="117041408"/>
-        <c:axId val="124391424"/>
+        <c:axId val="98566528"/>
+        <c:axId val="98568064"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="117041408"/>
+        <c:axId val="98566528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2672,7 +2760,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124391424"/>
+        <c:crossAx val="98568064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2680,7 +2768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124391424"/>
+        <c:axId val="98568064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2731,7 +2819,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117041408"/>
+        <c:crossAx val="98566528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2745,7 +2833,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3395,7 +3482,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91579B79-405D-485C-98E4-87124039E2F2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91579B79-405D-485C-98E4-87124039E2F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3705,7 +3792,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9126,41 +9213,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:U150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="8">
         <v>16</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="8">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="8">
         <v>16</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="8">
         <v>4</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="8">
         <v>4</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="8">
         <v>16</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="8">
         <v>20</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="8">
         <v>16</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="8">
         <v>32</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="8">
         <v>16</v>
       </c>
     </row>
@@ -9275,22 +9364,22 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P21" si="8">ROUNDDOWN((O3 * P$1 / O$1), 0)</f>
+        <f t="shared" ref="P3:P19" si="8">ROUNDDOWN((O3 * P$1 / O$1), 0)</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q21" si="9">ROUNDDOWN(((O3 + 1) * P$1 / O$1), 0) - 1</f>
+        <f t="shared" ref="Q3:Q19" si="9">ROUNDDOWN(((O3 + 1) * P$1 / O$1), 0) - 1</f>
         <v>0</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T33" si="10">ROUNDDOWN((S3 * T$1 / S$1), 0)</f>
+        <f t="shared" ref="T3:T19" si="10">ROUNDDOWN((S3 * T$1 / S$1), 0)</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U33" si="11">ROUNDDOWN(((S3 + 1) * T$1 / S$1), 0) - 1</f>
+        <f t="shared" ref="U3:U19" si="11">ROUNDDOWN(((S3 + 1) * T$1 / S$1), 0) - 1</f>
         <v>0</v>
       </c>
     </row>
@@ -10244,59 +10333,87 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
+        <f>1024/A21</f>
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <f>1-(A20/C20)</f>
+        <v>0.87450980392156863</v>
+      </c>
+      <c r="C20" s="7">
         <v>255</v>
+      </c>
+      <c r="E20" s="9">
+        <v>32</v>
+      </c>
+      <c r="F20" s="10">
+        <v>32</v>
+      </c>
+      <c r="G20" s="11">
+        <f>F20*E20</f>
+        <v>1024</v>
       </c>
       <c r="O20">
         <v>18</v>
       </c>
       <c r="P20">
-        <f t="shared" si="8"/>
+        <f>ROUNDDOWN((O20 * P$1 / O$1), 0)</f>
         <v>14</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="9"/>
+        <f>ROUNDDOWN(((O20 + 1) * P$1 / O$1), 0) - 1</f>
         <v>14</v>
       </c>
       <c r="S20">
         <v>18</v>
       </c>
       <c r="T20">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S20 * T$1 / S$1), 0)</f>
         <v>9</v>
       </c>
       <c r="U20">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S20 + 1) * T$1 / S$1), 0) - 1</f>
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="8">
         <v>32</v>
       </c>
-      <c r="B21">
-        <f>A20 * (1 - (A$21/A$20))</f>
+      <c r="C21" s="7">
+        <f>ROUNDDOWN(C20 * B$20,0)</f>
         <v>223</v>
+      </c>
+      <c r="E21" s="12">
+        <v>64</v>
+      </c>
+      <c r="F21" s="13">
+        <v>16</v>
+      </c>
+      <c r="G21" s="14">
+        <f t="shared" ref="G21:G24" si="17">F21*E21</f>
+        <v>1024</v>
       </c>
       <c r="O21">
         <v>19</v>
       </c>
       <c r="P21">
-        <f t="shared" si="8"/>
+        <f>ROUNDDOWN((O21 * P$1 / O$1), 0)</f>
         <v>15</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="9"/>
+        <f>ROUNDDOWN(((O21 + 1) * P$1 / O$1), 0) - 1</f>
         <v>15</v>
       </c>
       <c r="S21">
         <v>19</v>
       </c>
       <c r="T21">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S21 * T$1 / S$1), 0)</f>
         <v>9</v>
       </c>
       <c r="U21">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S21 + 1) * T$1 / S$1), 0) - 1</f>
         <v>9</v>
       </c>
     </row>
@@ -10305,455 +10422,1449 @@
         <f>A21-1</f>
         <v>31</v>
       </c>
-      <c r="B22">
-        <f t="shared" ref="B22:B53" si="17">A21 * (1 - (A$21/A$20))</f>
-        <v>27.984313725490196</v>
+      <c r="C22" s="7">
+        <f t="shared" ref="C22:C87" si="18">ROUNDDOWN(C21 * B$20,0)</f>
+        <v>195</v>
+      </c>
+      <c r="E22" s="12">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13">
+        <v>64</v>
+      </c>
+      <c r="G22" s="14">
+        <f t="shared" si="17"/>
+        <v>1024</v>
       </c>
       <c r="S22">
         <v>20</v>
       </c>
       <c r="T22">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S22 * T$1 / S$1), 0)</f>
         <v>10</v>
       </c>
       <c r="U22">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S22 + 1) * T$1 / S$1), 0) - 1</f>
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ref="A23:A36" si="18">A22-1</f>
+        <f t="shared" ref="A23:A36" si="19">A22-1</f>
         <v>30</v>
       </c>
-      <c r="B23">
+      <c r="C23" s="7">
+        <f t="shared" si="18"/>
+        <v>170</v>
+      </c>
+      <c r="E23" s="12">
+        <v>128</v>
+      </c>
+      <c r="F23" s="13">
+        <v>8</v>
+      </c>
+      <c r="G23" s="14">
         <f t="shared" si="17"/>
-        <v>27.109803921568627</v>
+        <v>1024</v>
       </c>
       <c r="S23">
         <v>21</v>
       </c>
       <c r="T23">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S23 * T$1 / S$1), 0)</f>
         <v>10</v>
       </c>
       <c r="U23">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S23 + 1) * T$1 / S$1), 0) - 1</f>
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
+        <f t="shared" si="19"/>
+        <v>29</v>
+      </c>
+      <c r="C24" s="7">
         <f t="shared" si="18"/>
-        <v>29</v>
-      </c>
-      <c r="B24">
+        <v>148</v>
+      </c>
+      <c r="E24" s="15">
+        <v>8</v>
+      </c>
+      <c r="F24" s="16">
+        <v>128</v>
+      </c>
+      <c r="G24" s="17">
         <f t="shared" si="17"/>
-        <v>26.235294117647058</v>
+        <v>1024</v>
       </c>
       <c r="S24">
         <v>22</v>
       </c>
       <c r="T24">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S24 * T$1 / S$1), 0)</f>
         <v>11</v>
       </c>
       <c r="U24">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S24 + 1) * T$1 / S$1), 0) - 1</f>
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
+        <f t="shared" si="19"/>
+        <v>28</v>
+      </c>
+      <c r="C25" s="7">
         <f t="shared" si="18"/>
-        <v>28</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="17"/>
-        <v>25.360784313725489</v>
+        <v>129</v>
       </c>
       <c r="S25">
         <v>23</v>
       </c>
       <c r="T25">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S25 * T$1 / S$1), 0)</f>
         <v>11</v>
       </c>
       <c r="U25">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S25 + 1) * T$1 / S$1), 0) - 1</f>
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
+        <f t="shared" si="19"/>
+        <v>27</v>
+      </c>
+      <c r="C26" s="7">
         <f t="shared" si="18"/>
-        <v>27</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="17"/>
-        <v>24.48627450980392</v>
+        <v>112</v>
       </c>
       <c r="S26">
         <v>24</v>
       </c>
       <c r="T26">
-        <f t="shared" si="10"/>
+        <f>ROUNDDOWN((S26 * T$1 / S$1), 0)</f>
         <v>12</v>
       </c>
       <c r="U26">
-        <f t="shared" si="11"/>
+        <f>ROUNDDOWN(((S26 + 1) * T$1 / S$1), 0) - 1</f>
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
+        <f t="shared" si="19"/>
+        <v>26</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="18"/>
+        <v>97</v>
+      </c>
+      <c r="S27">
+        <v>25</v>
+      </c>
+      <c r="T27">
+        <f>ROUNDDOWN((S27 * T$1 / S$1), 0)</f>
+        <v>12</v>
+      </c>
+      <c r="U27">
+        <f>ROUNDDOWN(((S27 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="18"/>
+        <v>84</v>
+      </c>
+      <c r="S28">
+        <v>26</v>
+      </c>
+      <c r="T28">
+        <f>ROUNDDOWN((S28 * T$1 / S$1), 0)</f>
+        <v>13</v>
+      </c>
+      <c r="U28">
+        <f>ROUNDDOWN(((S28 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="19"/>
+        <v>24</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="18"/>
+        <v>73</v>
+      </c>
+      <c r="S29">
+        <v>27</v>
+      </c>
+      <c r="T29">
+        <f>ROUNDDOWN((S29 * T$1 / S$1), 0)</f>
+        <v>13</v>
+      </c>
+      <c r="U29">
+        <f>ROUNDDOWN(((S29 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="19"/>
+        <v>23</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="18"/>
+        <v>63</v>
+      </c>
+      <c r="S30">
+        <v>28</v>
+      </c>
+      <c r="T30">
+        <f>ROUNDDOWN((S30 * T$1 / S$1), 0)</f>
+        <v>14</v>
+      </c>
+      <c r="U30">
+        <f>ROUNDDOWN(((S30 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="19"/>
+        <v>22</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="18"/>
+        <v>55</v>
+      </c>
+      <c r="S31">
+        <v>29</v>
+      </c>
+      <c r="T31">
+        <f>ROUNDDOWN((S31 * T$1 / S$1), 0)</f>
+        <v>14</v>
+      </c>
+      <c r="U31">
+        <f>ROUNDDOWN(((S31 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="19"/>
+        <v>21</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="18"/>
+        <v>48</v>
+      </c>
+      <c r="S32">
+        <v>30</v>
+      </c>
+      <c r="T32">
+        <f>ROUNDDOWN((S32 * T$1 / S$1), 0)</f>
+        <v>15</v>
+      </c>
+      <c r="U32">
+        <f>ROUNDDOWN(((S32 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="19"/>
+        <v>20</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="18"/>
+        <v>41</v>
+      </c>
+      <c r="S33">
+        <v>31</v>
+      </c>
+      <c r="T33">
+        <f>ROUNDDOWN((S33 * T$1 / S$1), 0)</f>
+        <v>15</v>
+      </c>
+      <c r="U33">
+        <f>ROUNDDOWN(((S33 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="19"/>
+        <v>19</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="18"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="19"/>
+        <v>18</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="18"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="19"/>
+        <v>17</v>
+      </c>
+      <c r="C36" s="7">
         <f t="shared" si="18"/>
         <v>26</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="17"/>
-        <v>23.611764705882354</v>
-      </c>
-      <c r="S27">
-        <v>25</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="11"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="18"/>
-        <v>25</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="17"/>
-        <v>22.737254901960785</v>
-      </c>
-      <c r="S28">
-        <v>26</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="11"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="18"/>
-        <v>24</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="17"/>
-        <v>21.862745098039216</v>
-      </c>
-      <c r="S29">
-        <v>27</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="18"/>
-        <v>23</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="17"/>
-        <v>20.988235294117647</v>
-      </c>
-      <c r="S30">
-        <v>28</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31">
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" ref="A37" si="20">A36-1</f>
+        <v>16</v>
+      </c>
+      <c r="C37" s="7">
         <f t="shared" si="18"/>
         <v>22</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="17"/>
-        <v>20.113725490196078</v>
-      </c>
-      <c r="S31">
-        <v>29</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="18"/>
-        <v>21</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="17"/>
-        <v>19.239215686274509</v>
-      </c>
-      <c r="S32">
-        <v>30</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="10"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" ref="A38:A51" si="21">A37-1</f>
         <v>15</v>
       </c>
-      <c r="U32">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="18"/>
-        <v>20</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="17"/>
-        <v>18.36470588235294</v>
-      </c>
-      <c r="S33">
-        <v>31</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="11"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="C38" s="7">
         <f t="shared" si="18"/>
         <v>19</v>
       </c>
-      <c r="B34">
-        <f t="shared" si="17"/>
-        <v>17.490196078431374</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="18"/>
-        <v>18</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="17"/>
-        <v>16.615686274509805</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="18"/>
-        <v>17</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="17"/>
-        <v>15.741176470588236</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" ref="A37" si="19">A36-1</f>
-        <v>16</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="17"/>
-        <v>14.866666666666667</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f t="shared" ref="A38:A51" si="20">A37-1</f>
-        <v>15</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="17"/>
-        <v>13.992156862745098</v>
-      </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>14</v>
       </c>
-      <c r="B39">
-        <f t="shared" si="17"/>
-        <v>13.117647058823529</v>
+      <c r="C39" s="7">
+        <f t="shared" si="18"/>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="B40">
-        <f t="shared" si="17"/>
-        <v>12.24313725490196</v>
+      <c r="C40" s="7">
+        <f t="shared" si="18"/>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="B41">
-        <f t="shared" si="17"/>
-        <v>11.368627450980393</v>
+      <c r="C41" s="7">
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
-      <c r="B42">
-        <f t="shared" si="17"/>
-        <v>10.494117647058824</v>
+      <c r="C42" s="7">
+        <f t="shared" si="18"/>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
-      <c r="B43">
-        <f t="shared" si="17"/>
-        <v>9.6196078431372545</v>
+      <c r="C43" s="7">
+        <f t="shared" si="18"/>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
-      <c r="B44">
-        <f t="shared" si="17"/>
-        <v>8.7450980392156872</v>
+      <c r="C44" s="7">
+        <f t="shared" si="18"/>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="B45">
-        <f t="shared" si="17"/>
-        <v>7.8705882352941181</v>
+      <c r="C45" s="7">
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="B46">
-        <f t="shared" si="17"/>
-        <v>6.996078431372549</v>
+      <c r="C46" s="7">
+        <f t="shared" si="18"/>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6</v>
       </c>
-      <c r="B47">
-        <f t="shared" si="17"/>
-        <v>6.12156862745098</v>
+      <c r="C47" s="7">
+        <f t="shared" si="18"/>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>5</v>
       </c>
-      <c r="B48">
-        <f t="shared" si="17"/>
-        <v>5.2470588235294118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="7">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
-      <c r="B49">
-        <f t="shared" si="17"/>
-        <v>4.3725490196078436</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="7">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
-      <c r="B50">
-        <f t="shared" si="17"/>
-        <v>3.4980392156862745</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="B51">
-        <f t="shared" si="17"/>
-        <v>2.6235294117647059</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" ref="A52:A53" si="21">A51-1</f>
+        <f t="shared" ref="A52:A85" si="22">A51-1</f>
         <v>1</v>
       </c>
-      <c r="B52">
-        <f t="shared" si="17"/>
-        <v>1.7490196078431373</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="17"/>
-        <v>0.87450980392156863</v>
-      </c>
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="22"/>
+        <v>-1</v>
+      </c>
+      <c r="C54" s="7">
+        <f>ROUNDDOWN(C53 * B$20,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="22"/>
+        <v>-2</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="22"/>
+        <v>-3</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="22"/>
+        <v>-4</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="22"/>
+        <v>-5</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="22"/>
+        <v>-6</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="22"/>
+        <v>-7</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="22"/>
+        <v>-8</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="22"/>
+        <v>-9</v>
+      </c>
+      <c r="C62" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="22"/>
+        <v>-10</v>
+      </c>
+      <c r="C63" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="22"/>
+        <v>-11</v>
+      </c>
+      <c r="C64" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="22"/>
+        <v>-12</v>
+      </c>
+      <c r="C65" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="22"/>
+        <v>-13</v>
+      </c>
+      <c r="C66" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="22"/>
+        <v>-14</v>
+      </c>
+      <c r="C67" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="22"/>
+        <v>-15</v>
+      </c>
+      <c r="C68" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="22"/>
+        <v>-16</v>
+      </c>
+      <c r="C69" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="22"/>
+        <v>-17</v>
+      </c>
+      <c r="C70" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="22"/>
+        <v>-18</v>
+      </c>
+      <c r="C71" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="22"/>
+        <v>-19</v>
+      </c>
+      <c r="C72" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="22"/>
+        <v>-20</v>
+      </c>
+      <c r="C73" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="22"/>
+        <v>-21</v>
+      </c>
+      <c r="C74" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="22"/>
+        <v>-22</v>
+      </c>
+      <c r="C75" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="22"/>
+        <v>-23</v>
+      </c>
+      <c r="C76" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="22"/>
+        <v>-24</v>
+      </c>
+      <c r="C77" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="22"/>
+        <v>-25</v>
+      </c>
+      <c r="C78" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="22"/>
+        <v>-26</v>
+      </c>
+      <c r="C79" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="22"/>
+        <v>-27</v>
+      </c>
+      <c r="C80" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="22"/>
+        <v>-28</v>
+      </c>
+      <c r="C81" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="22"/>
+        <v>-29</v>
+      </c>
+      <c r="C82" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="22"/>
+        <v>-30</v>
+      </c>
+      <c r="C83" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="22"/>
+        <v>-31</v>
+      </c>
+      <c r="C84" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="22"/>
+        <v>-32</v>
+      </c>
+      <c r="C85" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f>A85-1</f>
+        <v>-33</v>
+      </c>
+      <c r="C86" s="7">
+        <f>ROUNDDOWN(C85 * B$20,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f>A86-1</f>
+        <v>-34</v>
+      </c>
+      <c r="C87" s="7">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" ref="A88:A150" si="23">A87-1</f>
+        <v>-35</v>
+      </c>
+      <c r="C88" s="7">
+        <f t="shared" ref="C88:C150" si="24">ROUNDDOWN(C87 * B$20,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="23"/>
+        <v>-36</v>
+      </c>
+      <c r="C89" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="23"/>
+        <v>-37</v>
+      </c>
+      <c r="C90" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="23"/>
+        <v>-38</v>
+      </c>
+      <c r="C91" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="23"/>
+        <v>-39</v>
+      </c>
+      <c r="C92" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="23"/>
+        <v>-40</v>
+      </c>
+      <c r="C93" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="23"/>
+        <v>-41</v>
+      </c>
+      <c r="C94" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="23"/>
+        <v>-42</v>
+      </c>
+      <c r="C95" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="23"/>
+        <v>-43</v>
+      </c>
+      <c r="C96" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="23"/>
+        <v>-44</v>
+      </c>
+      <c r="C97" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f t="shared" si="23"/>
+        <v>-45</v>
+      </c>
+      <c r="C98" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f t="shared" si="23"/>
+        <v>-46</v>
+      </c>
+      <c r="C99" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f t="shared" si="23"/>
+        <v>-47</v>
+      </c>
+      <c r="C100" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <f t="shared" si="23"/>
+        <v>-48</v>
+      </c>
+      <c r="C101" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <f t="shared" si="23"/>
+        <v>-49</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f t="shared" si="23"/>
+        <v>-50</v>
+      </c>
+      <c r="C103" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <f t="shared" si="23"/>
+        <v>-51</v>
+      </c>
+      <c r="C104" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <f t="shared" si="23"/>
+        <v>-52</v>
+      </c>
+      <c r="C105" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <f t="shared" si="23"/>
+        <v>-53</v>
+      </c>
+      <c r="C106" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <f t="shared" si="23"/>
+        <v>-54</v>
+      </c>
+      <c r="C107" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <f t="shared" si="23"/>
+        <v>-55</v>
+      </c>
+      <c r="C108" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <f t="shared" si="23"/>
+        <v>-56</v>
+      </c>
+      <c r="C109" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <f t="shared" si="23"/>
+        <v>-57</v>
+      </c>
+      <c r="C110" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <f t="shared" si="23"/>
+        <v>-58</v>
+      </c>
+      <c r="C111" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <f t="shared" si="23"/>
+        <v>-59</v>
+      </c>
+      <c r="C112" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <f t="shared" si="23"/>
+        <v>-60</v>
+      </c>
+      <c r="C113" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <f t="shared" si="23"/>
+        <v>-61</v>
+      </c>
+      <c r="C114" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <f t="shared" si="23"/>
+        <v>-62</v>
+      </c>
+      <c r="C115" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <f t="shared" si="23"/>
+        <v>-63</v>
+      </c>
+      <c r="C116" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <f t="shared" si="23"/>
+        <v>-64</v>
+      </c>
+      <c r="C117" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <f t="shared" si="23"/>
+        <v>-65</v>
+      </c>
+      <c r="C118" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <f t="shared" si="23"/>
+        <v>-66</v>
+      </c>
+      <c r="C119" s="7">
+        <f>ROUNDDOWN(C118 * B$20,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <f t="shared" si="23"/>
+        <v>-67</v>
+      </c>
+      <c r="C120" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <f t="shared" si="23"/>
+        <v>-68</v>
+      </c>
+      <c r="C121" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <f t="shared" si="23"/>
+        <v>-69</v>
+      </c>
+      <c r="C122" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <f t="shared" si="23"/>
+        <v>-70</v>
+      </c>
+      <c r="C123" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <f t="shared" si="23"/>
+        <v>-71</v>
+      </c>
+      <c r="C124" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <f t="shared" si="23"/>
+        <v>-72</v>
+      </c>
+      <c r="C125" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <f t="shared" si="23"/>
+        <v>-73</v>
+      </c>
+      <c r="C126" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <f t="shared" si="23"/>
+        <v>-74</v>
+      </c>
+      <c r="C127" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <f t="shared" si="23"/>
+        <v>-75</v>
+      </c>
+      <c r="C128" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <f t="shared" si="23"/>
+        <v>-76</v>
+      </c>
+      <c r="C129" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <f t="shared" si="23"/>
+        <v>-77</v>
+      </c>
+      <c r="C130" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <f t="shared" si="23"/>
+        <v>-78</v>
+      </c>
+      <c r="C131" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <f t="shared" si="23"/>
+        <v>-79</v>
+      </c>
+      <c r="C132" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <f t="shared" si="23"/>
+        <v>-80</v>
+      </c>
+      <c r="C133" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <f t="shared" si="23"/>
+        <v>-81</v>
+      </c>
+      <c r="C134" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f t="shared" si="23"/>
+        <v>-82</v>
+      </c>
+      <c r="C135" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <f t="shared" si="23"/>
+        <v>-83</v>
+      </c>
+      <c r="C136" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <f t="shared" si="23"/>
+        <v>-84</v>
+      </c>
+      <c r="C137" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <f t="shared" si="23"/>
+        <v>-85</v>
+      </c>
+      <c r="C138" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <f t="shared" si="23"/>
+        <v>-86</v>
+      </c>
+      <c r="C139" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <f t="shared" si="23"/>
+        <v>-87</v>
+      </c>
+      <c r="C140" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <f t="shared" si="23"/>
+        <v>-88</v>
+      </c>
+      <c r="C141" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <f t="shared" si="23"/>
+        <v>-89</v>
+      </c>
+      <c r="C142" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <f t="shared" si="23"/>
+        <v>-90</v>
+      </c>
+      <c r="C143" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <f t="shared" si="23"/>
+        <v>-91</v>
+      </c>
+      <c r="C144" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <f t="shared" si="23"/>
+        <v>-92</v>
+      </c>
+      <c r="C145" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <f t="shared" si="23"/>
+        <v>-93</v>
+      </c>
+      <c r="C146" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <f t="shared" si="23"/>
+        <v>-94</v>
+      </c>
+      <c r="C147" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <f t="shared" si="23"/>
+        <v>-95</v>
+      </c>
+      <c r="C148" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <f t="shared" si="23"/>
+        <v>-96</v>
+      </c>
+      <c r="C149" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10761,7 +11872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10813,35 +11924,35 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <f>A3+B$2</f>
+        <f t="shared" ref="B3:B34" si="0">A3+B$2</f>
         <v>4</v>
       </c>
       <c r="C3" s="3">
-        <f>IF(B3&gt;=$A$2, B3 - $A$2, IF(B3&lt;0, B3 + $A$2, B3))</f>
+        <f t="shared" ref="C3:C34" si="1">IF(B3&gt;=$A$2, B3 - $A$2, IF(B3&lt;0, B3 + $A$2, B3))</f>
         <v>4</v>
       </c>
       <c r="D3" s="2">
-        <f>ROUNDDOWN(A3/2,0)</f>
+        <f t="shared" ref="D3:D34" si="2">ROUNDDOWN(A3/2,0)</f>
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <f>$A$2-D3 - 1</f>
+        <f t="shared" ref="E3:E34" si="3">$A$2-D3 - 1</f>
         <v>31</v>
       </c>
       <c r="F3" s="2">
-        <f>D3+B$2</f>
+        <f t="shared" ref="F3:F34" si="4">D3+B$2</f>
         <v>4</v>
       </c>
       <c r="G3" s="2">
-        <f>E3+B$2</f>
+        <f t="shared" ref="G3:G34" si="5">E3+B$2</f>
         <v>35</v>
       </c>
       <c r="H3" s="2">
-        <f>IF(F3&gt;=$A$2, F3 - $A$2, IF(F3&lt;0, F3 + $A$2, F3))</f>
+        <f t="shared" ref="H3:H34" si="6">IF(F3&gt;=$A$2, F3 - $A$2, IF(F3&lt;0, F3 + $A$2, F3))</f>
         <v>4</v>
       </c>
       <c r="I3" s="2">
-        <f>IF(G3&gt;=$A$2, G3 - $A$2, IF(G3&lt;0, G3 + $A$2, G3))</f>
+        <f t="shared" ref="I3:I34" si="7">IF(G3&gt;=$A$2, G3 - $A$2, IF(G3&lt;0, G3 + $A$2, G3))</f>
         <v>3</v>
       </c>
     </row>
@@ -10850,35 +11961,35 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <f>A4+B$2</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <f>IF(B4&gt;=$A$2, B4 - $A$2, IF(B4&lt;0, B4 + $A$2, B4))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <f>ROUNDDOWN(A4/2,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <f>$A$2-D4 - 1</f>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="F4" s="2">
-        <f>D4+B$2</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G4" s="2">
-        <f>E4+B$2</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="H4" s="2">
-        <f>IF(F4&gt;=$A$2, F4 - $A$2, IF(F4&lt;0, F4 + $A$2, F4))</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I4" s="2">
-        <f>IF(G4&gt;=$A$2, G4 - $A$2, IF(G4&lt;0, G4 + $A$2, G4))</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
@@ -10887,35 +11998,35 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <f>A5+B$2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <f>IF(B5&gt;=$A$2, B5 - $A$2, IF(B5&lt;0, B5 + $A$2, B5))</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <f>ROUNDDOWN(A5/2,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f>$A$2-D5 - 1</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="F5" s="2">
-        <f>D5+B$2</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G5" s="2">
-        <f>E5+B$2</f>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="H5" s="2">
-        <f>IF(F5&gt;=$A$2, F5 - $A$2, IF(F5&lt;0, F5 + $A$2, F5))</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I5" s="2">
-        <f>IF(G5&gt;=$A$2, G5 - $A$2, IF(G5&lt;0, G5 + $A$2, G5))</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
@@ -10924,35 +12035,35 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <f>A6+B$2</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C6" s="3">
-        <f>IF(B6&gt;=$A$2, B6 - $A$2, IF(B6&lt;0, B6 + $A$2, B6))</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="D6" s="2">
-        <f>ROUNDDOWN(A6/2,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <f>$A$2-D6 - 1</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="F6" s="2">
-        <f>D6+B$2</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G6" s="2">
-        <f>E6+B$2</f>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="H6" s="2">
-        <f>IF(F6&gt;=$A$2, F6 - $A$2, IF(F6&lt;0, F6 + $A$2, F6))</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I6" s="2">
-        <f>IF(G6&gt;=$A$2, G6 - $A$2, IF(G6&lt;0, G6 + $A$2, G6))</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
@@ -10961,35 +12072,35 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <f>A7+B$2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C7" s="3">
-        <f>IF(B7&gt;=$A$2, B7 - $A$2, IF(B7&lt;0, B7 + $A$2, B7))</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="D7" s="2">
-        <f>ROUNDDOWN(A7/2,0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <f>$A$2-D7 - 1</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="F7" s="2">
-        <f>D7+B$2</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="G7" s="2">
-        <f>E7+B$2</f>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="H7" s="2">
-        <f>IF(F7&gt;=$A$2, F7 - $A$2, IF(F7&lt;0, F7 + $A$2, F7))</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I7" s="2">
-        <f>IF(G7&gt;=$A$2, G7 - $A$2, IF(G7&lt;0, G7 + $A$2, G7))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -10998,35 +12109,35 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <f>A8+B$2</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C8" s="3">
-        <f>IF(B8&gt;=$A$2, B8 - $A$2, IF(B8&lt;0, B8 + $A$2, B8))</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="D8" s="2">
-        <f>ROUNDDOWN(A8/2,0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E8" s="2">
-        <f>$A$2-D8 - 1</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="F8" s="2">
-        <f>D8+B$2</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="G8" s="2">
-        <f>E8+B$2</f>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="H8" s="2">
-        <f>IF(F8&gt;=$A$2, F8 - $A$2, IF(F8&lt;0, F8 + $A$2, F8))</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I8" s="2">
-        <f>IF(G8&gt;=$A$2, G8 - $A$2, IF(G8&lt;0, G8 + $A$2, G8))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11035,35 +12146,35 @@
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <f>A9+B$2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C9" s="3">
-        <f>IF(B9&gt;=$A$2, B9 - $A$2, IF(B9&lt;0, B9 + $A$2, B9))</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="D9" s="2">
-        <f>ROUNDDOWN(A9/2,0)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E9" s="2">
-        <f>$A$2-D9 - 1</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="F9" s="2">
-        <f>D9+B$2</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G9" s="2">
-        <f>E9+B$2</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="H9" s="2">
-        <f>IF(F9&gt;=$A$2, F9 - $A$2, IF(F9&lt;0, F9 + $A$2, F9))</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I9" s="2">
-        <f>IF(G9&gt;=$A$2, G9 - $A$2, IF(G9&lt;0, G9 + $A$2, G9))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -11072,35 +12183,35 @@
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <f>A10+B$2</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C10" s="3">
-        <f>IF(B10&gt;=$A$2, B10 - $A$2, IF(B10&lt;0, B10 + $A$2, B10))</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="D10" s="2">
-        <f>ROUNDDOWN(A10/2,0)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E10" s="2">
-        <f>$A$2-D10 - 1</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="F10" s="2">
-        <f>D10+B$2</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G10" s="2">
-        <f>E10+B$2</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="H10" s="2">
-        <f>IF(F10&gt;=$A$2, F10 - $A$2, IF(F10&lt;0, F10 + $A$2, F10))</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I10" s="2">
-        <f>IF(G10&gt;=$A$2, G10 - $A$2, IF(G10&lt;0, G10 + $A$2, G10))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -11109,35 +12220,35 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <f>A11+B$2</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C11" s="3">
-        <f>IF(B11&gt;=$A$2, B11 - $A$2, IF(B11&lt;0, B11 + $A$2, B11))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="D11" s="2">
-        <f>ROUNDDOWN(A11/2,0)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E11" s="2">
-        <f>$A$2-D11 - 1</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="F11" s="2">
-        <f>D11+B$2</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G11" s="2">
-        <f>E11+B$2</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="H11" s="2">
-        <f>IF(F11&gt;=$A$2, F11 - $A$2, IF(F11&lt;0, F11 + $A$2, F11))</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="I11" s="2">
-        <f>IF(G11&gt;=$A$2, G11 - $A$2, IF(G11&lt;0, G11 + $A$2, G11))</f>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
     </row>
@@ -11146,35 +12257,35 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <f>A12+B$2</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C12" s="3">
-        <f>IF(B12&gt;=$A$2, B12 - $A$2, IF(B12&lt;0, B12 + $A$2, B12))</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="D12" s="2">
-        <f>ROUNDDOWN(A12/2,0)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E12" s="2">
-        <f>$A$2-D12 - 1</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="F12" s="2">
-        <f>D12+B$2</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G12" s="2">
-        <f>E12+B$2</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="H12" s="2">
-        <f>IF(F12&gt;=$A$2, F12 - $A$2, IF(F12&lt;0, F12 + $A$2, F12))</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="I12" s="2">
-        <f>IF(G12&gt;=$A$2, G12 - $A$2, IF(G12&lt;0, G12 + $A$2, G12))</f>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
     </row>
@@ -11183,35 +12294,35 @@
         <v>10</v>
       </c>
       <c r="B13" s="2">
-        <f>A13+B$2</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C13" s="3">
-        <f>IF(B13&gt;=$A$2, B13 - $A$2, IF(B13&lt;0, B13 + $A$2, B13))</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="D13" s="2">
-        <f>ROUNDDOWN(A13/2,0)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E13" s="2">
-        <f>$A$2-D13 - 1</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="F13" s="2">
-        <f>D13+B$2</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G13" s="2">
-        <f>E13+B$2</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="H13" s="2">
-        <f>IF(F13&gt;=$A$2, F13 - $A$2, IF(F13&lt;0, F13 + $A$2, F13))</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="I13" s="2">
-        <f>IF(G13&gt;=$A$2, G13 - $A$2, IF(G13&lt;0, G13 + $A$2, G13))</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
     </row>
@@ -11220,35 +12331,35 @@
         <v>11</v>
       </c>
       <c r="B14" s="2">
-        <f>A14+B$2</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C14" s="3">
-        <f>IF(B14&gt;=$A$2, B14 - $A$2, IF(B14&lt;0, B14 + $A$2, B14))</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D14" s="2">
-        <f>ROUNDDOWN(A14/2,0)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E14" s="2">
-        <f>$A$2-D14 - 1</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="F14" s="2">
-        <f>D14+B$2</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G14" s="2">
-        <f>E14+B$2</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="H14" s="2">
-        <f>IF(F14&gt;=$A$2, F14 - $A$2, IF(F14&lt;0, F14 + $A$2, F14))</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="I14" s="2">
-        <f>IF(G14&gt;=$A$2, G14 - $A$2, IF(G14&lt;0, G14 + $A$2, G14))</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
     </row>
@@ -11257,35 +12368,35 @@
         <v>12</v>
       </c>
       <c r="B15" s="2">
-        <f>A15+B$2</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C15" s="3">
-        <f>IF(B15&gt;=$A$2, B15 - $A$2, IF(B15&lt;0, B15 + $A$2, B15))</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="D15" s="2">
-        <f>ROUNDDOWN(A15/2,0)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E15" s="2">
-        <f>$A$2-D15 - 1</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="F15" s="2">
-        <f>D15+B$2</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G15" s="2">
-        <f>E15+B$2</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="H15" s="2">
-        <f>IF(F15&gt;=$A$2, F15 - $A$2, IF(F15&lt;0, F15 + $A$2, F15))</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="I15" s="2">
-        <f>IF(G15&gt;=$A$2, G15 - $A$2, IF(G15&lt;0, G15 + $A$2, G15))</f>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
     </row>
@@ -11294,35 +12405,35 @@
         <v>13</v>
       </c>
       <c r="B16" s="2">
-        <f>A16+B$2</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C16" s="3">
-        <f>IF(B16&gt;=$A$2, B16 - $A$2, IF(B16&lt;0, B16 + $A$2, B16))</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="D16" s="2">
-        <f>ROUNDDOWN(A16/2,0)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E16" s="2">
-        <f>$A$2-D16 - 1</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="F16" s="2">
-        <f>D16+B$2</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G16" s="2">
-        <f>E16+B$2</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="H16" s="2">
-        <f>IF(F16&gt;=$A$2, F16 - $A$2, IF(F16&lt;0, F16 + $A$2, F16))</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="I16" s="2">
-        <f>IF(G16&gt;=$A$2, G16 - $A$2, IF(G16&lt;0, G16 + $A$2, G16))</f>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
     </row>
@@ -11331,35 +12442,35 @@
         <v>14</v>
       </c>
       <c r="B17" s="2">
-        <f>A17+B$2</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C17" s="3">
-        <f>IF(B17&gt;=$A$2, B17 - $A$2, IF(B17&lt;0, B17 + $A$2, B17))</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D17" s="2">
-        <f>ROUNDDOWN(A17/2,0)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E17" s="2">
-        <f>$A$2-D17 - 1</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="F17" s="2">
-        <f>D17+B$2</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G17" s="2">
-        <f>E17+B$2</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="H17" s="2">
-        <f>IF(F17&gt;=$A$2, F17 - $A$2, IF(F17&lt;0, F17 + $A$2, F17))</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="I17" s="2">
-        <f>IF(G17&gt;=$A$2, G17 - $A$2, IF(G17&lt;0, G17 + $A$2, G17))</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
     </row>
@@ -11368,35 +12479,35 @@
         <v>15</v>
       </c>
       <c r="B18" s="2">
-        <f>A18+B$2</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C18" s="3">
-        <f>IF(B18&gt;=$A$2, B18 - $A$2, IF(B18&lt;0, B18 + $A$2, B18))</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="D18" s="2">
-        <f>ROUNDDOWN(A18/2,0)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E18" s="2">
-        <f>$A$2-D18 - 1</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="F18" s="2">
-        <f>D18+B$2</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G18" s="2">
-        <f>E18+B$2</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="H18" s="2">
-        <f>IF(F18&gt;=$A$2, F18 - $A$2, IF(F18&lt;0, F18 + $A$2, F18))</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="I18" s="2">
-        <f>IF(G18&gt;=$A$2, G18 - $A$2, IF(G18&lt;0, G18 + $A$2, G18))</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
     </row>
@@ -11405,35 +12516,35 @@
         <v>16</v>
       </c>
       <c r="B19" s="2">
-        <f>A19+B$2</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <f>IF(B19&gt;=$A$2, B19 - $A$2, IF(B19&lt;0, B19 + $A$2, B19))</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D19" s="2">
-        <f>ROUNDDOWN(A19/2,0)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E19" s="2">
-        <f>$A$2-D19 - 1</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="F19" s="2">
-        <f>D19+B$2</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G19" s="2">
-        <f>E19+B$2</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="H19" s="2">
-        <f>IF(F19&gt;=$A$2, F19 - $A$2, IF(F19&lt;0, F19 + $A$2, F19))</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="I19" s="2">
-        <f>IF(G19&gt;=$A$2, G19 - $A$2, IF(G19&lt;0, G19 + $A$2, G19))</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
     </row>
@@ -11442,35 +12553,35 @@
         <v>17</v>
       </c>
       <c r="B20" s="2">
-        <f>A20+B$2</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C20" s="3">
-        <f>IF(B20&gt;=$A$2, B20 - $A$2, IF(B20&lt;0, B20 + $A$2, B20))</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="D20" s="2">
-        <f>ROUNDDOWN(A20/2,0)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E20" s="2">
-        <f>$A$2-D20 - 1</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="F20" s="2">
-        <f>D20+B$2</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G20" s="2">
-        <f>E20+B$2</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="H20" s="2">
-        <f>IF(F20&gt;=$A$2, F20 - $A$2, IF(F20&lt;0, F20 + $A$2, F20))</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="I20" s="2">
-        <f>IF(G20&gt;=$A$2, G20 - $A$2, IF(G20&lt;0, G20 + $A$2, G20))</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
     </row>
@@ -11479,35 +12590,35 @@
         <v>18</v>
       </c>
       <c r="B21" s="2">
-        <f>A21+B$2</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C21" s="3">
-        <f>IF(B21&gt;=$A$2, B21 - $A$2, IF(B21&lt;0, B21 + $A$2, B21))</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="D21" s="2">
-        <f>ROUNDDOWN(A21/2,0)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E21" s="2">
-        <f>$A$2-D21 - 1</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="F21" s="2">
-        <f>D21+B$2</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G21" s="2">
-        <f>E21+B$2</f>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="H21" s="2">
-        <f>IF(F21&gt;=$A$2, F21 - $A$2, IF(F21&lt;0, F21 + $A$2, F21))</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="I21" s="2">
-        <f>IF(G21&gt;=$A$2, G21 - $A$2, IF(G21&lt;0, G21 + $A$2, G21))</f>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
     </row>
@@ -11516,35 +12627,35 @@
         <v>19</v>
       </c>
       <c r="B22" s="2">
-        <f>A22+B$2</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C22" s="3">
-        <f>IF(B22&gt;=$A$2, B22 - $A$2, IF(B22&lt;0, B22 + $A$2, B22))</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D22" s="2">
-        <f>ROUNDDOWN(A22/2,0)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E22" s="2">
-        <f>$A$2-D22 - 1</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="F22" s="2">
-        <f>D22+B$2</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G22" s="2">
-        <f>E22+B$2</f>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="H22" s="2">
-        <f>IF(F22&gt;=$A$2, F22 - $A$2, IF(F22&lt;0, F22 + $A$2, F22))</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="I22" s="2">
-        <f>IF(G22&gt;=$A$2, G22 - $A$2, IF(G22&lt;0, G22 + $A$2, G22))</f>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
     </row>
@@ -11553,35 +12664,35 @@
         <v>20</v>
       </c>
       <c r="B23" s="2">
-        <f>A23+B$2</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C23" s="3">
-        <f>IF(B23&gt;=$A$2, B23 - $A$2, IF(B23&lt;0, B23 + $A$2, B23))</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="D23" s="2">
-        <f>ROUNDDOWN(A23/2,0)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E23" s="2">
-        <f>$A$2-D23 - 1</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <f>D23+B$2</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G23" s="2">
-        <f>E23+B$2</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="H23" s="2">
-        <f>IF(F23&gt;=$A$2, F23 - $A$2, IF(F23&lt;0, F23 + $A$2, F23))</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="I23" s="2">
-        <f>IF(G23&gt;=$A$2, G23 - $A$2, IF(G23&lt;0, G23 + $A$2, G23))</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
     </row>
@@ -11590,35 +12701,35 @@
         <v>21</v>
       </c>
       <c r="B24" s="2">
-        <f>A24+B$2</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C24" s="3">
-        <f>IF(B24&gt;=$A$2, B24 - $A$2, IF(B24&lt;0, B24 + $A$2, B24))</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D24" s="2">
-        <f>ROUNDDOWN(A24/2,0)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E24" s="2">
-        <f>$A$2-D24 - 1</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="F24" s="2">
-        <f>D24+B$2</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G24" s="2">
-        <f>E24+B$2</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="H24" s="2">
-        <f>IF(F24&gt;=$A$2, F24 - $A$2, IF(F24&lt;0, F24 + $A$2, F24))</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="I24" s="2">
-        <f>IF(G24&gt;=$A$2, G24 - $A$2, IF(G24&lt;0, G24 + $A$2, G24))</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
     </row>
@@ -11627,35 +12738,35 @@
         <v>22</v>
       </c>
       <c r="B25" s="2">
-        <f>A25+B$2</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C25" s="3">
-        <f>IF(B25&gt;=$A$2, B25 - $A$2, IF(B25&lt;0, B25 + $A$2, B25))</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="D25" s="2">
-        <f>ROUNDDOWN(A25/2,0)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E25" s="2">
-        <f>$A$2-D25 - 1</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="F25" s="2">
-        <f>D25+B$2</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G25" s="2">
-        <f>E25+B$2</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="H25" s="2">
-        <f>IF(F25&gt;=$A$2, F25 - $A$2, IF(F25&lt;0, F25 + $A$2, F25))</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I25" s="2">
-        <f>IF(G25&gt;=$A$2, G25 - $A$2, IF(G25&lt;0, G25 + $A$2, G25))</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
     </row>
@@ -11664,35 +12775,35 @@
         <v>23</v>
       </c>
       <c r="B26" s="2">
-        <f>A26+B$2</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C26" s="3">
-        <f>IF(B26&gt;=$A$2, B26 - $A$2, IF(B26&lt;0, B26 + $A$2, B26))</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="D26" s="2">
-        <f>ROUNDDOWN(A26/2,0)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E26" s="2">
-        <f>$A$2-D26 - 1</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="F26" s="2">
-        <f>D26+B$2</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G26" s="2">
-        <f>E26+B$2</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="H26" s="2">
-        <f>IF(F26&gt;=$A$2, F26 - $A$2, IF(F26&lt;0, F26 + $A$2, F26))</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I26" s="2">
-        <f>IF(G26&gt;=$A$2, G26 - $A$2, IF(G26&lt;0, G26 + $A$2, G26))</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
     </row>
@@ -11701,35 +12812,35 @@
         <v>24</v>
       </c>
       <c r="B27" s="2">
-        <f>A27+B$2</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C27" s="3">
-        <f>IF(B27&gt;=$A$2, B27 - $A$2, IF(B27&lt;0, B27 + $A$2, B27))</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="D27" s="2">
-        <f>ROUNDDOWN(A27/2,0)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E27" s="2">
-        <f>$A$2-D27 - 1</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="F27" s="2">
-        <f>D27+B$2</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G27" s="2">
-        <f>E27+B$2</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="H27" s="2">
-        <f>IF(F27&gt;=$A$2, F27 - $A$2, IF(F27&lt;0, F27 + $A$2, F27))</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="I27" s="2">
-        <f>IF(G27&gt;=$A$2, G27 - $A$2, IF(G27&lt;0, G27 + $A$2, G27))</f>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
     </row>
@@ -11738,35 +12849,35 @@
         <v>25</v>
       </c>
       <c r="B28" s="2">
-        <f>A28+B$2</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C28" s="3">
-        <f>IF(B28&gt;=$A$2, B28 - $A$2, IF(B28&lt;0, B28 + $A$2, B28))</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="D28" s="2">
-        <f>ROUNDDOWN(A28/2,0)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E28" s="2">
-        <f>$A$2-D28 - 1</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="F28" s="2">
-        <f>D28+B$2</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G28" s="2">
-        <f>E28+B$2</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="H28" s="2">
-        <f>IF(F28&gt;=$A$2, F28 - $A$2, IF(F28&lt;0, F28 + $A$2, F28))</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="I28" s="2">
-        <f>IF(G28&gt;=$A$2, G28 - $A$2, IF(G28&lt;0, G28 + $A$2, G28))</f>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
     </row>
@@ -11775,35 +12886,35 @@
         <v>26</v>
       </c>
       <c r="B29" s="2">
-        <f>A29+B$2</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C29" s="3">
-        <f>IF(B29&gt;=$A$2, B29 - $A$2, IF(B29&lt;0, B29 + $A$2, B29))</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D29" s="2">
-        <f>ROUNDDOWN(A29/2,0)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E29" s="2">
-        <f>$A$2-D29 - 1</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="F29" s="2">
-        <f>D29+B$2</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G29" s="2">
-        <f>E29+B$2</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="H29" s="2">
-        <f>IF(F29&gt;=$A$2, F29 - $A$2, IF(F29&lt;0, F29 + $A$2, F29))</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="I29" s="2">
-        <f>IF(G29&gt;=$A$2, G29 - $A$2, IF(G29&lt;0, G29 + $A$2, G29))</f>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
     </row>
@@ -11812,35 +12923,35 @@
         <v>27</v>
       </c>
       <c r="B30" s="2">
-        <f>A30+B$2</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C30" s="3">
-        <f>IF(B30&gt;=$A$2, B30 - $A$2, IF(B30&lt;0, B30 + $A$2, B30))</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="D30" s="2">
-        <f>ROUNDDOWN(A30/2,0)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E30" s="2">
-        <f>$A$2-D30 - 1</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="F30" s="2">
-        <f>D30+B$2</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G30" s="2">
-        <f>E30+B$2</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="H30" s="2">
-        <f>IF(F30&gt;=$A$2, F30 - $A$2, IF(F30&lt;0, F30 + $A$2, F30))</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="I30" s="2">
-        <f>IF(G30&gt;=$A$2, G30 - $A$2, IF(G30&lt;0, G30 + $A$2, G30))</f>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
     </row>
@@ -11849,35 +12960,35 @@
         <v>28</v>
       </c>
       <c r="B31" s="2">
-        <f>A31+B$2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C31" s="3">
-        <f>IF(B31&gt;=$A$2, B31 - $A$2, IF(B31&lt;0, B31 + $A$2, B31))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31" s="2">
-        <f>ROUNDDOWN(A31/2,0)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E31" s="2">
-        <f>$A$2-D31 - 1</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="F31" s="2">
-        <f>D31+B$2</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G31" s="2">
-        <f>E31+B$2</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="H31" s="2">
-        <f>IF(F31&gt;=$A$2, F31 - $A$2, IF(F31&lt;0, F31 + $A$2, F31))</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="I31" s="2">
-        <f>IF(G31&gt;=$A$2, G31 - $A$2, IF(G31&lt;0, G31 + $A$2, G31))</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
     </row>
@@ -11886,35 +12997,35 @@
         <v>29</v>
       </c>
       <c r="B32" s="2">
-        <f>A32+B$2</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="C32" s="3">
-        <f>IF(B32&gt;=$A$2, B32 - $A$2, IF(B32&lt;0, B32 + $A$2, B32))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D32" s="2">
-        <f>ROUNDDOWN(A32/2,0)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E32" s="2">
-        <f>$A$2-D32 - 1</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="F32" s="2">
-        <f>D32+B$2</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G32" s="2">
-        <f>E32+B$2</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="H32" s="2">
-        <f>IF(F32&gt;=$A$2, F32 - $A$2, IF(F32&lt;0, F32 + $A$2, F32))</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="I32" s="2">
-        <f>IF(G32&gt;=$A$2, G32 - $A$2, IF(G32&lt;0, G32 + $A$2, G32))</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
     </row>
@@ -11923,35 +13034,35 @@
         <v>30</v>
       </c>
       <c r="B33" s="2">
-        <f>A33+B$2</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="C33" s="3">
-        <f>IF(B33&gt;=$A$2, B33 - $A$2, IF(B33&lt;0, B33 + $A$2, B33))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D33" s="2">
-        <f>ROUNDDOWN(A33/2,0)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="E33" s="2">
-        <f>$A$2-D33 - 1</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F33" s="2">
-        <f>D33+B$2</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="G33" s="2">
-        <f>E33+B$2</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="H33" s="2">
-        <f>IF(F33&gt;=$A$2, F33 - $A$2, IF(F33&lt;0, F33 + $A$2, F33))</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="I33" s="2">
-        <f>IF(G33&gt;=$A$2, G33 - $A$2, IF(G33&lt;0, G33 + $A$2, G33))</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
     </row>
@@ -11960,35 +13071,35 @@
         <v>31</v>
       </c>
       <c r="B34" s="2">
-        <f>A34+B$2</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="C34" s="3">
-        <f>IF(B34&gt;=$A$2, B34 - $A$2, IF(B34&lt;0, B34 + $A$2, B34))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D34" s="2">
-        <f>ROUNDDOWN(A34/2,0)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="E34" s="2">
-        <f>$A$2-D34 - 1</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F34" s="2">
-        <f>D34+B$2</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="G34" s="2">
-        <f>E34+B$2</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="H34" s="2">
-        <f>IF(F34&gt;=$A$2, F34 - $A$2, IF(F34&lt;0, F34 + $A$2, F34))</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="I34" s="2">
-        <f>IF(G34&gt;=$A$2, G34 - $A$2, IF(G34&lt;0, G34 + $A$2, G34))</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
     </row>

</xml_diff>